<commit_message>
cred and course update
</commit_message>
<xml_diff>
--- a/course-progress.xlsx
+++ b/course-progress.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\edu\aws_certified_developer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7127634-92C4-4321-87A9-0251FF701460}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{429E6FCD-2771-4BA4-ADDB-1D968B0A877E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29565" yWindow="4095" windowWidth="21585" windowHeight="11895" xr2:uid="{8B6F4BBE-1A5D-4E09-B9F0-402EB90B90D8}"/>
+    <workbookView xWindow="29565" yWindow="3705" windowWidth="21585" windowHeight="11895" xr2:uid="{8B6F4BBE-1A5D-4E09-B9F0-402EB90B90D8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,18 +33,51 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>% Complete Goal</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Goal Date</t>
   </si>
   <si>
-    <t>% Complete Actual</t>
-  </si>
-  <si>
     <t>AWS Certified Developer Course</t>
+  </si>
+  <si>
+    <t>Skill level: All Levels</t>
+  </si>
+  <si>
+    <t>Students: 82452</t>
+  </si>
+  <si>
+    <t>Languages: English</t>
+  </si>
+  <si>
+    <t>Captions: Yes</t>
+  </si>
+  <si>
+    <t>Practice tests: 1</t>
+  </si>
+  <si>
+    <t>Questions: 65</t>
+  </si>
+  <si>
+    <t>Lectures: 221</t>
+  </si>
+  <si>
+    <t>Video: 19 total hours</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - need approx 2hrs of video per week to obtain goal</t>
+  </si>
+  <si>
+    <t>Goal Section</t>
+  </si>
+  <si>
+    <t>Actual Section Complete</t>
+  </si>
+  <si>
+    <t>Actual % Complete</t>
+  </si>
+  <si>
+    <t>Goal % Complete</t>
   </si>
 </sst>
 </file>
@@ -52,7 +85,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -117,16 +150,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -441,159 +480,258 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAEF5432-6327-45A4-8007-9599E8A569E6}">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="22.140625" style="1"/>
+    <col min="3" max="3" width="22.140625" style="12"/>
+    <col min="4" max="4" width="24.5703125" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+    <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
+        <v>0</v>
+      </c>
+      <c r="B4" s="5">
+        <v>43892</v>
+      </c>
+      <c r="C4" s="11">
+        <v>0</v>
+      </c>
+      <c r="D4" s="8">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="5">
-        <v>0</v>
-      </c>
-      <c r="B4" s="6">
-        <v>43892</v>
-      </c>
-      <c r="C4" s="5">
+      <c r="E4" s="4">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
         <f>SUM(A4 + 10)</f>
         <v>10</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5" s="5">
         <f>SUM(B4 + 7)</f>
         <v>43899</v>
       </c>
-      <c r="C5" s="5"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="5">
+      <c r="C5" s="11">
+        <v>3</v>
+      </c>
+      <c r="D5" s="8"/>
+      <c r="E5" s="4"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
         <f t="shared" ref="A6:A14" si="0">SUM(A5 + 10)</f>
         <v>20</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6" s="5">
         <f t="shared" ref="B6:B14" si="1">SUM(B5 + 7)</f>
         <v>43906</v>
       </c>
-      <c r="C6" s="5"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="5">
+      <c r="C6" s="11">
+        <v>5</v>
+      </c>
+      <c r="D6" s="8"/>
+      <c r="E6" s="4"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B7" s="5">
         <f t="shared" si="1"/>
         <v>43913</v>
       </c>
-      <c r="C7" s="5"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="5">
+      <c r="C7" s="11">
+        <v>7</v>
+      </c>
+      <c r="D7" s="8"/>
+      <c r="E7" s="4"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-      <c r="B8" s="6">
+      <c r="B8" s="5">
         <f t="shared" si="1"/>
         <v>43920</v>
       </c>
-      <c r="C8" s="5"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="5">
+      <c r="C8" s="11">
+        <v>9.84</v>
+      </c>
+      <c r="D8" s="8"/>
+      <c r="E8" s="4"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="4">
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
-      <c r="B9" s="6">
+      <c r="B9" s="5">
         <f t="shared" si="1"/>
         <v>43927</v>
       </c>
-      <c r="C9" s="5"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="5">
+      <c r="C9" s="11">
+        <v>11.106</v>
+      </c>
+      <c r="D9" s="8"/>
+      <c r="E9" s="4"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="4">
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
-      <c r="B10" s="6">
+      <c r="B10" s="5">
         <f t="shared" si="1"/>
         <v>43934</v>
       </c>
-      <c r="C10" s="5"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="5">
+      <c r="C10" s="11">
+        <v>12</v>
+      </c>
+      <c r="D10" s="8"/>
+      <c r="E10" s="4"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="4">
         <f t="shared" si="0"/>
         <v>70</v>
       </c>
-      <c r="B11" s="6">
+      <c r="B11" s="5">
         <f t="shared" si="1"/>
         <v>43941</v>
       </c>
-      <c r="C11" s="5"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="5">
+      <c r="C11" s="11">
+        <v>14.148</v>
+      </c>
+      <c r="D11" s="8"/>
+      <c r="E11" s="4"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
         <f t="shared" si="0"/>
         <v>80</v>
       </c>
-      <c r="B12" s="6">
+      <c r="B12" s="5">
         <f t="shared" si="1"/>
         <v>43948</v>
       </c>
-      <c r="C12" s="5"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="5">
+      <c r="C12" s="11">
+        <v>16</v>
+      </c>
+      <c r="D12" s="8"/>
+      <c r="E12" s="4"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="4">
         <f t="shared" si="0"/>
         <v>90</v>
       </c>
-      <c r="B13" s="6">
+      <c r="B13" s="5">
         <f t="shared" si="1"/>
         <v>43955</v>
       </c>
-      <c r="C13" s="5"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="5">
+      <c r="C13" s="11">
+        <v>18</v>
+      </c>
+      <c r="D13" s="8"/>
+      <c r="E13" s="4"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="4">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="B14" s="6">
+      <c r="B14" s="5">
         <f t="shared" si="1"/>
         <v>43962</v>
       </c>
-      <c r="C14" s="5"/>
+      <c r="C14" s="11">
+        <v>22</v>
+      </c>
+      <c r="D14" s="8"/>
+      <c r="E14" s="4"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>2</v>
+      </c>
+      <c r="E17" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>9</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A1:E1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>